<commit_message>
Changes as per the new Export templates
</commit_message>
<xml_diff>
--- a/SKCE.Valuation.API/SKCE.Valuation.API/Export Templates/Export_Format_PG.xlsx
+++ b/SKCE.Valuation.API/SKCE.Valuation.API/Export Templates/Export_Format_PG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SKCE\Workspace\SKCE.Valuation.API\SKCE.Valuation.API\Export Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B97815-B893-47BA-98C2-230211BA1BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AB5739-62D4-4EB4-9926-20DFB1CCDF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7364ED79-667F-4112-B629-800C0366CD85}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>11(i)</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>PART_A_TOTAL</t>
+  </si>
+  <si>
+    <t>COLLEGE_CODE</t>
+  </si>
+  <si>
+    <t>COURSE_CODE</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706801F3-E4E3-4BC8-A09B-489E7FEAAA43}">
-  <dimension ref="A1:AP1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -502,141 +508,149 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" customWidth="1"/>
-    <col min="38" max="38" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" customWidth="1"/>
+    <col min="40" max="40" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="3" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="3" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1">
+      <c r="E1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="1">
+      <c r="F1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1">
+      <c r="G1" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="1">
+      <c r="H1" s="1">
         <v>4</v>
       </c>
-      <c r="G1" s="1">
+      <c r="I1" s="1">
         <v>5</v>
       </c>
-      <c r="H1" s="1">
+      <c r="J1" s="1">
         <v>6</v>
       </c>
-      <c r="I1" s="1">
+      <c r="K1" s="1">
         <v>7</v>
       </c>
-      <c r="J1" s="1">
+      <c r="L1" s="1">
         <v>8</v>
       </c>
-      <c r="K1" s="1">
+      <c r="M1" s="1">
         <v>9</v>
       </c>
-      <c r="L1" s="1">
+      <c r="N1" s="1">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>